<commit_message>
Create CSV file with Classic answers
</commit_message>
<xml_diff>
--- a/Magic 8 Ball Answers.xlsx
+++ b/Magic 8 Ball Answers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Magic 8-Ball\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Magic 8 Ball\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5116FFE8-4DF3-451D-A68A-36ACED0F99C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D07289-0C71-4B4E-B134-9101633D6448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B918F773-97DF-407C-A83D-CAD1937955E1}"/>
+    <workbookView xWindow="28680" yWindow="-4125" windowWidth="29040" windowHeight="15840" xr2:uid="{B918F773-97DF-407C-A83D-CAD1937955E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Magic Answers" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,13 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -127,13 +134,13 @@
     <t>Without a doubt</t>
   </si>
   <si>
-    <t>Yes – definitely</t>
-  </si>
-  <si>
     <t>You may rely on it</t>
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Yes, definitely</t>
   </si>
 </sst>
 </file>
@@ -521,7 +528,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,7 +694,7 @@
         <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -695,12 +702,12 @@
         <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B22">
         <f>SUBTOTAL(103,Answers[Answer])</f>

</xml_diff>